<commit_message>
Update url linkage file
</commit_message>
<xml_diff>
--- a/myInfo/queryParameter_Linkage.xlsx
+++ b/myInfo/queryParameter_Linkage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB.Jaspo\myCCB\myInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\CCB UI Update\ui_update_app\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92982C4-1125-4FDF-90C8-79ACE934C0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77BB980-0B90-494D-B0C7-9E7FEAD5C1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{D3A4EB56-BD7B-4DE5-B361-4DC1FFA4D382}"/>
   </bookViews>
@@ -1032,9 +1032,6 @@
     <t>educationTrendTab</t>
   </si>
   <si>
-    <t>lifeExpectancyTab</t>
-  </si>
-  <si>
     <t>ranks</t>
   </si>
   <si>
@@ -1152,10 +1149,13 @@
     <t>LEADING CAUSES TREND</t>
   </si>
   <si>
-    <t>topTrendsTab</t>
-  </si>
-  <si>
     <t>leadingcausestrend</t>
+  </si>
+  <si>
+    <t>lifeExpectancyTrendTab</t>
+  </si>
+  <si>
+    <t>leadingCausesTrendTab</t>
   </si>
 </sst>
 </file>
@@ -1509,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F50DBCD-5A3C-4AED-A7E8-75EA46ECE524}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,13 +1552,13 @@
         <v>304</v>
       </c>
       <c r="C3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D3" t="s">
         <v>339</v>
       </c>
-      <c r="D3" t="s">
-        <v>340</v>
-      </c>
       <c r="E3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1569,13 +1569,13 @@
         <v>305</v>
       </c>
       <c r="C4" t="s">
+        <v>331</v>
+      </c>
+      <c r="D4" t="s">
         <v>332</v>
       </c>
-      <c r="D4" t="s">
-        <v>333</v>
-      </c>
       <c r="E4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1586,13 +1586,13 @@
         <v>306</v>
       </c>
       <c r="C5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1603,13 +1603,13 @@
         <v>307</v>
       </c>
       <c r="C6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1620,13 +1620,13 @@
         <v>308</v>
       </c>
       <c r="C7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1637,13 +1637,13 @@
         <v>309</v>
       </c>
       <c r="C8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1654,13 +1654,13 @@
         <v>310</v>
       </c>
       <c r="C9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1677,7 +1677,7 @@
         <v>327</v>
       </c>
       <c r="E10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
         <v>328</v>
       </c>
       <c r="E11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1711,7 +1711,7 @@
         <v>329</v>
       </c>
       <c r="E12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1728,7 +1728,7 @@
         <v>330</v>
       </c>
       <c r="E13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1742,10 +1742,10 @@
         <v>322</v>
       </c>
       <c r="D14" t="s">
-        <v>331</v>
+        <v>371</v>
       </c>
       <c r="E14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1753,16 +1753,16 @@
         <v>297</v>
       </c>
       <c r="B15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C15" t="s">
         <v>322</v>
       </c>
       <c r="D15" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E15" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1776,7 +1776,7 @@
         <v>323</v>
       </c>
       <c r="D16" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E16" t="s">
         <v>323</v>
@@ -1793,7 +1793,7 @@
         <v>324</v>
       </c>
       <c r="D17" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E17" t="s">
         <v>324</v>
@@ -1810,10 +1810,10 @@
         <v>325</v>
       </c>
       <c r="D18" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1827,10 +1827,10 @@
         <v>325</v>
       </c>
       <c r="D19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1844,7 +1844,7 @@
         <v>326</v>
       </c>
       <c r="D20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E20" t="s">
         <v>326</v>
@@ -1863,13 +1863,13 @@
         <v>319</v>
       </c>
       <c r="C22" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1880,13 +1880,13 @@
         <v>320</v>
       </c>
       <c r="C23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D23" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E23" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1897,13 +1897,13 @@
         <v>321</v>
       </c>
       <c r="C24" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D24" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1911,16 +1911,16 @@
         <v>303</v>
       </c>
       <c r="B25" t="s">
+        <v>366</v>
+      </c>
+      <c r="C25" t="s">
+        <v>365</v>
+      </c>
+      <c r="D25" t="s">
         <v>367</v>
       </c>
-      <c r="C25" t="s">
-        <v>366</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>368</v>
-      </c>
-      <c r="E25" t="s">
-        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>